<commit_message>
Request; Worker; Server folder contains the latest working code.
</commit_message>
<xml_diff>
--- a/Other Files/Password Cracking Stats.xlsx
+++ b/Other Files/Password Cracking Stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="8595" windowHeight="3660"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="7110" windowHeight="3660"/>
   </bookViews>
   <sheets>
     <sheet name="Stat Trial 1" sheetId="1" r:id="rId1"/>
@@ -574,19 +574,19 @@
                   <c:v>27.257374316666667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>42.735919266666663</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>51.052184349999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>21.257617200000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>14.108057550000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>28.249680066666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -2403,19 +2403,19 @@
                   <c:v>27.257374316666667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>42.735919266666663</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>51.052184349999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>21.257617200000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>14.108057550000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>28.249680066666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -2528,7 +2528,7 @@
                   <c:v>509.92592535</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>60.616594233333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2779,19 +2779,19 @@
                   <c:v>27.945634183333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.76776656666666665</c:v>
+                  <c:v>43.503685833333329</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.87657083333333341</c:v>
+                  <c:v>51.92875518333333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.94242170000000003</c:v>
+                  <c:v>22.200038900000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.0064825500000001</c:v>
+                  <c:v>15.114540100000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.39157440000000004</c:v>
+                  <c:v>28.641254466666666</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.40366503333333331</c:v>
@@ -3328,8 +3328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3683,6 +3683,21 @@
       <c r="J9" s="2">
         <v>442459</v>
       </c>
+      <c r="K9" s="2">
+        <v>155156</v>
+      </c>
+      <c r="L9" s="2">
+        <v>131061</v>
+      </c>
+      <c r="M9" s="2">
+        <v>457032</v>
+      </c>
+      <c r="N9" s="2">
+        <v>483453</v>
+      </c>
+      <c r="O9" s="2">
+        <v>980804</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -3693,6 +3708,9 @@
       </c>
       <c r="C10" s="2">
         <v>555521</v>
+      </c>
+      <c r="D10" s="2">
+        <v>995654</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -4023,6 +4041,21 @@
       <c r="J19" s="2">
         <v>1635</v>
       </c>
+      <c r="K19" s="2">
+        <v>2564</v>
+      </c>
+      <c r="L19" s="2">
+        <v>3063</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1275</v>
+      </c>
+      <c r="N19" s="2">
+        <v>846</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1694</v>
+      </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -4033,6 +4066,9 @@
       </c>
       <c r="C20" s="2">
         <v>30595</v>
+      </c>
+      <c r="D20" s="2">
+        <v>3636</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -4434,23 +4470,23 @@
       </c>
       <c r="K29" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>42.735919266666663</v>
       </c>
       <c r="L29" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>51.052184349999997</v>
       </c>
       <c r="M29" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>21.257617200000002</v>
       </c>
       <c r="N29" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>14.108057550000002</v>
       </c>
       <c r="O29" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28.249680066666667</v>
       </c>
       <c r="P29" s="2">
         <f t="shared" si="3"/>
@@ -4491,7 +4527,7 @@
       </c>
       <c r="D30" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>60.616594233333331</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="4"/>
@@ -4771,23 +4807,23 @@
       </c>
       <c r="K33" s="4">
         <f t="shared" si="7"/>
-        <v>0.76776656666666665</v>
+        <v>43.503685833333329</v>
       </c>
       <c r="L33" s="4">
         <f t="shared" si="7"/>
-        <v>0.87657083333333341</v>
+        <v>51.92875518333333</v>
       </c>
       <c r="M33" s="4">
         <f t="shared" si="7"/>
-        <v>0.94242170000000003</v>
+        <v>22.200038900000003</v>
       </c>
       <c r="N33" s="4">
         <f t="shared" si="7"/>
-        <v>1.0064825500000001</v>
+        <v>15.114540100000001</v>
       </c>
       <c r="O33" s="4">
         <f t="shared" si="7"/>
-        <v>0.39157440000000004</v>
+        <v>28.641254466666666</v>
       </c>
       <c r="P33" s="4">
         <f t="shared" si="7"/>
@@ -5203,23 +5239,23 @@
       </c>
       <c r="K39" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.71226532111111107</v>
       </c>
       <c r="L39" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.85086973916666664</v>
       </c>
       <c r="M39" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.35429362000000003</v>
       </c>
       <c r="N39" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.23513429250000004</v>
       </c>
       <c r="O39" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.47082800111111112</v>
       </c>
       <c r="P39" s="2">
         <f t="shared" si="11"/>
@@ -5260,7 +5296,7 @@
       </c>
       <c r="D40" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1.0102765705555554</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="12"/>

</xml_diff>

<commit_message>
Fixed port number control for both server and clients
</commit_message>
<xml_diff>
--- a/Other Files/Password Cracking Stats.xlsx
+++ b/Other Files/Password Cracking Stats.xlsx
@@ -589,10 +589,10 @@
                   <c:v>28.249680066666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>28.410347183333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>28.12123561666667</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -2418,10 +2418,10 @@
                   <c:v>28.249680066666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>28.410347183333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>28.12123561666667</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -2794,10 +2794,10 @@
                   <c:v>28.641254466666666</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.40366503333333331</c:v>
+                  <c:v>28.814012216666665</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.52217463333333336</c:v>
+                  <c:v>28.643410250000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.45557838333333334</c:v>
@@ -3329,7 +3329,7 @@
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3698,6 +3698,12 @@
       <c r="O9" s="2">
         <v>980804</v>
       </c>
+      <c r="P9" s="2">
+        <v>620831</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>274137</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -4056,6 +4062,12 @@
       <c r="O19" s="2">
         <v>1694</v>
       </c>
+      <c r="P19" s="2">
+        <v>1704</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>1687</v>
+      </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -4490,11 +4502,11 @@
       </c>
       <c r="P29" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28.410347183333332</v>
       </c>
       <c r="Q29" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28.12123561666667</v>
       </c>
       <c r="R29" s="2">
         <f t="shared" si="3"/>
@@ -4827,11 +4839,11 @@
       </c>
       <c r="P33" s="4">
         <f t="shared" si="7"/>
-        <v>0.40366503333333331</v>
+        <v>28.814012216666665</v>
       </c>
       <c r="Q33" s="4">
         <f t="shared" si="7"/>
-        <v>0.52217463333333336</v>
+        <v>28.643410250000002</v>
       </c>
       <c r="R33" s="4">
         <f t="shared" si="7"/>
@@ -5259,11 +5271,11 @@
       </c>
       <c r="P39" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.47350578638888885</v>
       </c>
       <c r="Q39" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.46868726027777785</v>
       </c>
       <c r="R39" s="2">
         <f t="shared" si="11"/>

</xml_diff>